<commit_message>
adjustments of balances and bleeds
</commit_message>
<xml_diff>
--- a/Baseline_Engine/High_BPR_Turbofan_Cycle_Data.xlsx
+++ b/Baseline_Engine/High_BPR_Turbofan_Cycle_Data.xlsx
@@ -341,12 +341,24 @@
       <name val="Ubuntu"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0"/>
+        <bgColor theme="3" tint="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor theme="8" tint="0.39997558519241921"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -434,59 +446,67 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" quotePrefix="0" pivotButton="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" quotePrefix="0" pivotButton="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" quotePrefix="0" pivotButton="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1" quotePrefix="0" pivotButton="0"/>
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" quotePrefix="0" pivotButton="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1" quotePrefix="0" pivotButton="0">
       <alignment vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1" quotePrefix="0" pivotButton="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" quotePrefix="0" pivotButton="0"/>
-    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1" quotePrefix="0" pivotButton="0"/>
-    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1" quotePrefix="0" pivotButton="0">
+    <xf fontId="1" fillId="3" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" quotePrefix="0" pivotButton="0"/>
+    <xf fontId="1" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" quotePrefix="0" pivotButton="0"/>
+    <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1" quotePrefix="0" pivotButton="0"/>
+    <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1" quotePrefix="0" pivotButton="0">
       <alignment vertical="center"/>
     </xf>
+    <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1" quotePrefix="0" pivotButton="0"/>
+    <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1" quotePrefix="0" pivotButton="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="1" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="0" pivotButton="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="1" fillId="4" borderId="0" numFmtId="165" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" quotePrefix="0" pivotButton="0"/>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1" quotePrefix="0" pivotButton="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="1" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" quotePrefix="0" pivotButton="0"/>
+    <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1" quotePrefix="0" pivotButton="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="1" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" quotePrefix="0" pivotButton="0"/>
+    <xf fontId="0" fillId="0" borderId="3" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1" quotePrefix="0" pivotButton="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="1" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" quotePrefix="0" pivotButton="0"/>
+    <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1" quotePrefix="0" pivotButton="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" quotePrefix="0" pivotButton="0"/>
+    <xf fontId="1" fillId="8" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" quotePrefix="0" pivotButton="0"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1" quotePrefix="0" pivotButton="0"/>
+    <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFill="1" quotePrefix="0" pivotButton="0"/>
+    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" quotePrefix="0" pivotButton="0"/>
+    <xf fontId="0" fillId="8" borderId="0" numFmtId="0" xfId="0" applyFill="1" quotePrefix="0" pivotButton="0"/>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1" quotePrefix="0" pivotButton="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="0" pivotButton="0">
-      <alignment horizontal="left"/>
+    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1" quotePrefix="0" pivotButton="0">
+      <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="1" fillId="2" borderId="0" numFmtId="165" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" quotePrefix="0" pivotButton="0"/>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1" quotePrefix="0" pivotButton="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf fontId="1" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" quotePrefix="0" pivotButton="0"/>
-    <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1" quotePrefix="0" pivotButton="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf fontId="1" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" quotePrefix="0" pivotButton="0"/>
-    <xf fontId="0" fillId="0" borderId="3" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1" quotePrefix="0" pivotButton="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf fontId="1" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" quotePrefix="0" pivotButton="0"/>
-    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1" quotePrefix="0" pivotButton="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" quotePrefix="0" pivotButton="0"/>
-    <xf fontId="1" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" quotePrefix="0" pivotButton="0"/>
-    <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1" quotePrefix="0" pivotButton="0"/>
-    <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1" quotePrefix="0" pivotButton="0"/>
-    <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFill="1" quotePrefix="0" pivotButton="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="166" xfId="0" applyNumberFormat="1" quotePrefix="0" pivotButton="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="166" xfId="0" applyNumberFormat="1" quotePrefix="0" pivotButton="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="166" xfId="0" applyNumberFormat="1" quotePrefix="0" pivotButton="0"/>
-    <xf fontId="0" fillId="7" borderId="0" numFmtId="166" xfId="0" applyNumberFormat="1" applyFill="1" quotePrefix="0" pivotButton="0"/>
-    <xf fontId="0" fillId="7" borderId="0" numFmtId="166" xfId="0" applyNumberFormat="1" applyFill="1" quotePrefix="0" pivotButton="0">
+    <xf fontId="0" fillId="9" borderId="0" numFmtId="166" xfId="0" applyNumberFormat="1" applyFill="1" quotePrefix="0" pivotButton="0"/>
+    <xf fontId="0" fillId="9" borderId="0" numFmtId="166" xfId="0" applyNumberFormat="1" applyFill="1" quotePrefix="0" pivotButton="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" quotePrefix="0" pivotButton="0"/>
+    <xf fontId="0" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFill="1" quotePrefix="0" pivotButton="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,7 +528,7 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>225136</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>164522</xdr:rowOff>
+      <xdr:rowOff>164521</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
@@ -689,7 +709,7 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>588818</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>161636</xdr:rowOff>
+      <xdr:rowOff>161635</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
@@ -783,7 +803,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>28863</xdr:colOff>
+      <xdr:colOff>28862</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>57727</xdr:rowOff>
     </xdr:to>
@@ -1099,7 +1119,7 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>37522</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>161636</xdr:rowOff>
+      <xdr:rowOff>161635</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
@@ -1861,14 +1881,15 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A18" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
   <cols>
     <col customWidth="1" min="4" max="4" width="19.140625"/>
-    <col customWidth="1" min="5" max="5" width="13.28125"/>
+    <col customWidth="1" min="5" max="5" width="19.00390625"/>
+    <col customWidth="1" min="6" max="6" width="11.421875"/>
     <col bestFit="1" min="8" max="8" width="9.54296875"/>
     <col customWidth="1" min="9" max="9" width="12.421875"/>
     <col bestFit="1" min="10" max="10" width="21.23046875"/>
@@ -2180,7 +2201,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="3">
+      <c r="J11" s="6">
         <f>(H10-H12)/H10</f>
         <v>0.014998774609917479</v>
       </c>
@@ -2217,7 +2238,7 @@
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
-      <c r="L12" s="6">
+      <c r="L12" s="7">
         <f>(F12-F15)/F12</f>
         <v>0.29199680935921296</v>
       </c>
@@ -2231,46 +2252,46 @@
         <v>0.995</v>
       </c>
     </row>
-    <row r="13" s="7" customFormat="1" ht="15">
-      <c r="D13" s="8"/>
-      <c r="E13" s="6" t="s">
+    <row r="13" s="8" customFormat="1" ht="15">
+      <c r="D13" s="9"/>
+      <c r="E13" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="7">
         <v>18.053000000000001</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="7">
         <v>839.65999999999997</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="7">
         <v>1808.6130000000001</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="7">
         <v>1.726</v>
       </c>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6" t="s">
+      <c r="J13" s="7"/>
+      <c r="K13" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="L13" s="6">
+      <c r="L13" s="7">
         <f>(F13-F15)/F13</f>
         <v>0.26250484683986042</v>
       </c>
-      <c r="M13" s="6">
+      <c r="M13" s="7">
         <f>(Q37+Q36)*F12</f>
         <v>0.75219999999999998</v>
       </c>
-      <c r="N13" s="7">
+      <c r="N13" s="8">
         <f>(500-H12)/(H13-H12)</f>
         <v>0.22477324279830027</v>
       </c>
-      <c r="O13" s="7" t="s">
+      <c r="O13" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="P13" s="9" t="s">
+      <c r="P13" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q13" s="9">
+      <c r="Q13" s="11">
         <v>50</v>
       </c>
     </row>
@@ -2292,47 +2313,47 @@
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
     </row>
-    <row r="15" s="7" customFormat="1" ht="15">
-      <c r="A15" s="7">
+    <row r="15" s="8" customFormat="1" ht="15">
+      <c r="A15" s="8">
         <f>F12-F15</f>
         <v>5.4909999999999997</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="12">
         <v>31</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="7">
         <v>13.314</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="7">
         <v>839.65999999999997</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="7">
         <v>1808.6130000000001</v>
       </c>
-      <c r="I15" s="6"/>
-      <c r="J15" s="11">
+      <c r="I15" s="7"/>
+      <c r="J15" s="13">
         <f>(H15-H16)/H15</f>
         <v>0.040000265396743263</v>
       </c>
-      <c r="K15" s="6" t="s">
+      <c r="K15" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6">
+      <c r="L15" s="7"/>
+      <c r="M15" s="7">
         <f>(Q34+Q35)*F12</f>
         <v>4.7012499999999999</v>
       </c>
-      <c r="N15" s="6">
+      <c r="N15" s="7">
         <v>1</v>
       </c>
-      <c r="O15" s="6">
+      <c r="O15" s="7">
         <v>1</v>
       </c>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="9"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
     </row>
     <row r="16" ht="15">
       <c r="E16" s="1" t="s">
@@ -2401,13 +2422,13 @@
         <f>F23-F16</f>
         <v>5.4539999999999988</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="14" t="s">
         <v>46</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F18" s="15">
         <v>16.725999999999999</v>
       </c>
       <c r="G18" s="1">
@@ -2437,7 +2458,7 @@
         <f>A18-A17</f>
         <v>0.36599999999999966</v>
       </c>
-      <c r="D19" s="14"/>
+      <c r="D19" s="16"/>
       <c r="E19" s="1" t="s">
         <v>49</v>
       </c>
@@ -2465,11 +2486,11 @@
       </c>
     </row>
     <row r="20" ht="15">
-      <c r="D20" s="14"/>
+      <c r="D20" s="16"/>
       <c r="E20" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F20" s="15">
+      <c r="F20" s="17">
         <v>18.419</v>
       </c>
       <c r="G20" s="1">
@@ -2493,11 +2514,11 @@
       </c>
     </row>
     <row r="21" ht="15">
-      <c r="D21" s="16"/>
+      <c r="D21" s="18"/>
       <c r="E21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F21" s="17">
+      <c r="F21" s="19">
         <v>19.045000000000002</v>
       </c>
       <c r="G21" s="1">
@@ -2550,7 +2571,7 @@
       </c>
     </row>
     <row r="23" ht="15">
-      <c r="A23" s="18">
+      <c r="A23" s="20">
         <f>18.805*0.16</f>
         <v>3.0087999999999999</v>
       </c>
@@ -2558,11 +2579,11 @@
         <f>1-F18/F12</f>
         <v>0.11055570327040687</v>
       </c>
-      <c r="C23" s="19"/>
+      <c r="C23" s="21"/>
       <c r="E23" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="20">
+      <c r="F23" s="22">
         <v>19.170999999999999</v>
       </c>
       <c r="G23" s="1">
@@ -2588,18 +2609,18 @@
       </c>
     </row>
     <row r="24" ht="15">
-      <c r="A24" s="18"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
+      <c r="A24" s="20"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
       <c r="D24" t="s">
         <v>30</v>
       </c>
       <c r="E24" s="1"/>
-      <c r="F24" s="20"/>
+      <c r="F24" s="22"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
-      <c r="J24" s="3">
+      <c r="J24" s="23">
         <f>(H23-H25)/H23</f>
         <v>0.010005663583160339</v>
       </c>
@@ -2612,7 +2633,7 @@
       <c r="Q24" s="2"/>
     </row>
     <row r="25" ht="15">
-      <c r="A25" s="21">
+      <c r="A25" s="24">
         <f>18.805*0.09</f>
         <v>1.69245</v>
       </c>
@@ -2645,7 +2666,7 @@
       </c>
     </row>
     <row r="26" ht="15">
-      <c r="A26" s="22">
+      <c r="A26" s="25">
         <f>18.805*0.03333</f>
         <v>0.62677064999999998</v>
       </c>
@@ -2664,7 +2685,7 @@
       <c r="I26" s="1">
         <v>564.47199999999998</v>
       </c>
-      <c r="J26" s="3">
+      <c r="J26" s="23">
         <f>(H6-H26)/H6</f>
         <v>0.029997844700903244</v>
       </c>
@@ -2681,7 +2702,7 @@
       </c>
     </row>
     <row r="27" ht="15">
-      <c r="A27" s="23">
+      <c r="A27" s="26">
         <f>18.805*0.00667</f>
         <v>0.12542935</v>
       </c>
@@ -2892,7 +2913,7 @@
       <c r="P34" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="Q34" s="18">
+      <c r="Q34" s="20">
         <v>0.16</v>
       </c>
     </row>
@@ -2925,7 +2946,7 @@
       <c r="P35" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="Q35" s="21">
+      <c r="Q35" s="24">
         <v>0.089999999999999997</v>
       </c>
     </row>
@@ -2950,7 +2971,7 @@
       <c r="P36" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="Q36" s="22">
+      <c r="Q36" s="25">
         <v>0.033329999999999999</v>
       </c>
     </row>
@@ -2979,7 +3000,7 @@
       <c r="P37" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="Q37" s="23">
+      <c r="Q37" s="26">
         <v>0.0066699999999999997</v>
       </c>
     </row>
@@ -3117,7 +3138,7 @@
       <c r="E46" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F46" s="2">
+      <c r="F46" s="27">
         <v>0.97999999999999998</v>
       </c>
       <c r="G46" s="2"/>
@@ -3128,7 +3149,7 @@
       <c r="E47" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="F47" s="2">
+      <c r="F47" s="28">
         <v>0.98499999999999999</v>
       </c>
       <c r="G47" s="2"/>
@@ -3155,25 +3176,25 @@
       <c r="E50" s="1">
         <v>13.314</v>
       </c>
-      <c r="F50" s="24">
-        <f>E50+3.0088</f>
+      <c r="F50" s="29">
+        <f t="shared" ref="F50:F59" si="0">E50+3.0088</f>
         <v>16.322800000000001</v>
       </c>
       <c r="G50" s="2"/>
-      <c r="H50" s="25">
-        <f>E50+1.69245</f>
+      <c r="H50" s="30">
+        <f t="shared" ref="H50:H59" si="1">E50+1.69245</f>
         <v>15.006450000000001</v>
       </c>
       <c r="I50" s="2"/>
-      <c r="J50" s="24">
-        <f>E50+0.626771</f>
+      <c r="J50" s="29">
+        <f t="shared" ref="J50:J59" si="2">E50+0.626771</f>
         <v>13.940771</v>
       </c>
-      <c r="K50" s="26"/>
-      <c r="L50" s="26"/>
-      <c r="M50" s="26"/>
+      <c r="K50" s="29"/>
+      <c r="L50" s="29"/>
+      <c r="M50" s="29"/>
       <c r="P50">
-        <f>E50+0.125429</f>
+        <f t="shared" ref="P50:P59" si="3">E50+0.125429</f>
         <v>13.439429000000001</v>
       </c>
     </row>
@@ -3181,25 +3202,25 @@
       <c r="E51" s="1">
         <v>13.717000000000001</v>
       </c>
-      <c r="F51" s="27">
-        <f>E51+3.0088</f>
+      <c r="F51" s="31">
+        <f t="shared" si="0"/>
         <v>16.7258</v>
       </c>
       <c r="G51" s="2"/>
-      <c r="H51" s="25">
-        <f>E51+1.69245</f>
+      <c r="H51" s="30">
+        <f t="shared" si="1"/>
         <v>15.40945</v>
       </c>
       <c r="I51" s="2"/>
-      <c r="J51" s="24">
-        <f>E51+0.626771</f>
+      <c r="J51" s="29">
+        <f t="shared" si="2"/>
         <v>14.343771</v>
       </c>
-      <c r="K51" s="26"/>
-      <c r="L51" s="26"/>
-      <c r="M51" s="26"/>
+      <c r="K51" s="29"/>
+      <c r="L51" s="29"/>
+      <c r="M51" s="29"/>
       <c r="P51">
-        <f>E51+0.125429</f>
+        <f t="shared" si="3"/>
         <v>13.842429000000001</v>
       </c>
     </row>
@@ -3207,25 +3228,25 @@
       <c r="E52" s="1">
         <v>15.786</v>
       </c>
-      <c r="F52" s="24">
-        <f>E52+3.0088</f>
+      <c r="F52" s="29">
+        <f t="shared" si="0"/>
         <v>18.794799999999999</v>
       </c>
       <c r="G52" s="2"/>
-      <c r="H52" s="25">
-        <f>E52+1.69245</f>
+      <c r="H52" s="30">
+        <f t="shared" si="1"/>
         <v>17.478449999999999</v>
       </c>
       <c r="I52" s="2"/>
-      <c r="J52" s="24">
-        <f>E52+0.626771</f>
+      <c r="J52" s="29">
+        <f t="shared" si="2"/>
         <v>16.412770999999999</v>
       </c>
-      <c r="K52" s="26"/>
-      <c r="L52" s="26"/>
-      <c r="M52" s="26"/>
+      <c r="K52" s="29"/>
+      <c r="L52" s="29"/>
+      <c r="M52" s="29"/>
       <c r="P52">
-        <f>E52+0.125429</f>
+        <f t="shared" si="3"/>
         <v>15.911429</v>
       </c>
     </row>
@@ -3233,25 +3254,25 @@
       <c r="E53" s="1">
         <v>16.725999999999999</v>
       </c>
-      <c r="F53" s="24">
-        <f>E53+3.0088</f>
+      <c r="F53" s="29">
+        <f t="shared" si="0"/>
         <v>19.7348</v>
       </c>
       <c r="G53" s="2"/>
-      <c r="H53" s="28">
+      <c r="H53" s="32">
         <f>E53+1.69245</f>
         <v>18.41845</v>
       </c>
       <c r="I53" s="2"/>
-      <c r="J53" s="24">
-        <f>E53+0.626771</f>
+      <c r="J53" s="29">
+        <f t="shared" si="2"/>
         <v>17.352771000000001</v>
       </c>
-      <c r="K53" s="26"/>
-      <c r="L53" s="26"/>
-      <c r="M53" s="26"/>
+      <c r="K53" s="29"/>
+      <c r="L53" s="29"/>
+      <c r="M53" s="29"/>
       <c r="P53">
-        <f>E53+0.125429</f>
+        <f t="shared" si="3"/>
         <v>16.851429</v>
       </c>
     </row>
@@ -3259,25 +3280,25 @@
       <c r="E54" s="1">
         <v>16.725999999999999</v>
       </c>
-      <c r="F54" s="24">
-        <f>E54+3.0088</f>
+      <c r="F54" s="29">
+        <f t="shared" si="0"/>
         <v>19.7348</v>
       </c>
       <c r="G54" s="2"/>
-      <c r="H54" s="25">
-        <f>E54+1.69245</f>
+      <c r="H54" s="30">
+        <f t="shared" si="1"/>
         <v>18.41845</v>
       </c>
       <c r="I54" s="2"/>
-      <c r="J54" s="24">
-        <f>E54+0.626771</f>
+      <c r="J54" s="29">
+        <f t="shared" si="2"/>
         <v>17.352771000000001</v>
       </c>
-      <c r="K54" s="26"/>
-      <c r="L54" s="26"/>
-      <c r="M54" s="26"/>
+      <c r="K54" s="29"/>
+      <c r="L54" s="29"/>
+      <c r="M54" s="29"/>
       <c r="P54">
-        <f>E54+0.125429</f>
+        <f t="shared" si="3"/>
         <v>16.851429</v>
       </c>
     </row>
@@ -3285,25 +3306,25 @@
       <c r="E55" s="1">
         <v>18.419</v>
       </c>
-      <c r="F55" s="24">
-        <f>E55+3.0088</f>
+      <c r="F55" s="29">
+        <f t="shared" si="0"/>
         <v>21.427800000000001</v>
       </c>
       <c r="G55" s="2"/>
-      <c r="H55" s="25">
-        <f>E55+1.69245</f>
+      <c r="H55" s="30">
+        <f t="shared" si="1"/>
         <v>20.111450000000001</v>
       </c>
       <c r="I55" s="2"/>
-      <c r="J55" s="27">
-        <f>E55+0.626771</f>
+      <c r="J55" s="31">
+        <f t="shared" si="2"/>
         <v>19.045771000000002</v>
       </c>
-      <c r="K55" s="26"/>
-      <c r="L55" s="26"/>
-      <c r="M55" s="26"/>
+      <c r="K55" s="29"/>
+      <c r="L55" s="29"/>
+      <c r="M55" s="29"/>
       <c r="P55">
-        <f>E55+0.125429</f>
+        <f t="shared" si="3"/>
         <v>18.544429000000001</v>
       </c>
     </row>
@@ -3311,25 +3332,25 @@
       <c r="E56" s="1">
         <v>19.045000000000002</v>
       </c>
-      <c r="F56" s="24">
-        <f>E56+3.0088</f>
+      <c r="F56" s="29">
+        <f t="shared" si="0"/>
         <v>22.053800000000003</v>
       </c>
       <c r="G56" s="2"/>
-      <c r="H56" s="25">
-        <f>E56+1.69245</f>
+      <c r="H56" s="30">
+        <f t="shared" si="1"/>
         <v>20.737450000000003</v>
       </c>
       <c r="I56" s="2"/>
-      <c r="J56" s="24">
-        <f>E56+0.626771</f>
+      <c r="J56" s="29">
+        <f t="shared" si="2"/>
         <v>19.671771000000003</v>
       </c>
-      <c r="K56" s="26"/>
-      <c r="L56" s="26"/>
-      <c r="M56" s="26"/>
-      <c r="P56" s="29">
-        <f>E56+0.125429</f>
+      <c r="K56" s="29"/>
+      <c r="L56" s="29"/>
+      <c r="M56" s="29"/>
+      <c r="P56" s="33">
+        <f t="shared" si="3"/>
         <v>19.170429000000002</v>
       </c>
     </row>
@@ -3337,25 +3358,25 @@
       <c r="E57" s="1">
         <v>19.045000000000002</v>
       </c>
-      <c r="F57" s="24">
-        <f>E57+3.0088</f>
+      <c r="F57" s="29">
+        <f t="shared" si="0"/>
         <v>22.053800000000003</v>
       </c>
       <c r="G57" s="2"/>
-      <c r="H57" s="25">
-        <f>E57+1.69245</f>
+      <c r="H57" s="30">
+        <f t="shared" si="1"/>
         <v>20.737450000000003</v>
       </c>
       <c r="I57" s="2"/>
-      <c r="J57" s="24">
-        <f>E57+0.626771</f>
+      <c r="J57" s="29">
+        <f t="shared" si="2"/>
         <v>19.671771000000003</v>
       </c>
-      <c r="K57" s="26"/>
-      <c r="L57" s="26"/>
-      <c r="M57" s="26"/>
+      <c r="K57" s="29"/>
+      <c r="L57" s="29"/>
+      <c r="M57" s="29"/>
       <c r="P57">
-        <f>E57+0.125429</f>
+        <f t="shared" si="3"/>
         <v>19.170429000000002</v>
       </c>
     </row>
@@ -3363,25 +3384,25 @@
       <c r="E58" s="1">
         <v>19.170999999999999</v>
       </c>
-      <c r="F58" s="24">
-        <f>E58+3.0088</f>
+      <c r="F58" s="29">
+        <f t="shared" si="0"/>
         <v>22.1798</v>
       </c>
       <c r="G58" s="2"/>
-      <c r="H58" s="25">
-        <f>E58+1.69245</f>
+      <c r="H58" s="30">
+        <f t="shared" si="1"/>
         <v>20.86345</v>
       </c>
       <c r="I58" s="2"/>
-      <c r="J58" s="24">
-        <f>E58+0.626771</f>
+      <c r="J58" s="29">
+        <f t="shared" si="2"/>
         <v>19.797771000000001</v>
       </c>
-      <c r="K58" s="26"/>
-      <c r="L58" s="26"/>
-      <c r="M58" s="26"/>
+      <c r="K58" s="29"/>
+      <c r="L58" s="29"/>
+      <c r="M58" s="29"/>
       <c r="P58">
-        <f>E58+0.125429</f>
+        <f t="shared" si="3"/>
         <v>19.296429</v>
       </c>
     </row>
@@ -3389,25 +3410,25 @@
       <c r="E59" s="1">
         <v>19.170999999999999</v>
       </c>
-      <c r="F59" s="24">
-        <f>E59+3.0088</f>
+      <c r="F59" s="29">
+        <f t="shared" si="0"/>
         <v>22.1798</v>
       </c>
       <c r="G59" s="2"/>
-      <c r="H59" s="25">
-        <f>E59+1.69245</f>
+      <c r="H59" s="30">
+        <f t="shared" si="1"/>
         <v>20.86345</v>
       </c>
       <c r="I59" s="2"/>
-      <c r="J59" s="24">
-        <f>E59+0.626771</f>
+      <c r="J59" s="29">
+        <f t="shared" si="2"/>
         <v>19.797771000000001</v>
       </c>
-      <c r="K59" s="26"/>
-      <c r="L59" s="26"/>
-      <c r="M59" s="26"/>
+      <c r="K59" s="29"/>
+      <c r="L59" s="29"/>
+      <c r="M59" s="29"/>
       <c r="P59">
-        <f>E59+0.125429</f>
+        <f t="shared" si="3"/>
         <v>19.296429</v>
       </c>
     </row>

</xml_diff>